<commit_message>
fiks in chart, ya Allah lancarkan sidang hamba
</commit_message>
<xml_diff>
--- a/database/nutristandard/bbu_boys.xlsx
+++ b/database/nutristandard/bbu_boys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester 8 (2025)\skripsi\Referensi\website posyandu\WHO growth standard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\posyandu-meneh-ki\database\nutristandard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24512444-7401-4949-AAA9-F468096F46C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8657667B-0393-4D37-A6C8-CC3E193BFADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Month</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>SD1</t>
+  </si>
+  <si>
+    <t>SD3neg</t>
+  </si>
+  <si>
+    <t>SD2neg</t>
+  </si>
+  <si>
+    <t>SD2</t>
+  </si>
+  <si>
+    <t>SD3</t>
   </si>
 </sst>
 </file>
@@ -872,880 +884,1624 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>2.1</v>
+      </c>
+      <c r="C2">
+        <v>2.5</v>
+      </c>
+      <c r="D2">
         <v>2.9</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>3.3</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>2.9</v>
+      </c>
+      <c r="C3">
+        <v>3.4</v>
+      </c>
+      <c r="D3">
         <v>3.9</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>4.5</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>5.8</v>
+      </c>
+      <c r="H3">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>3.8</v>
+      </c>
+      <c r="C4">
+        <v>4.3</v>
+      </c>
+      <c r="D4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>5.6</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>7.1</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
         <v>5.7</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>6.4</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C6">
+        <v>5.6</v>
+      </c>
+      <c r="D6">
         <v>6.2</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>7</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H6">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
+        <v>5.3</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
         <v>6.7</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>7.5</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H7">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
+        <v>5.7</v>
+      </c>
+      <c r="C8">
+        <v>6.4</v>
+      </c>
+      <c r="D8">
         <v>7.1</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>7.9</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="H8">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
+        <v>5.9</v>
+      </c>
+      <c r="C9">
+        <v>6.7</v>
+      </c>
+      <c r="D9">
         <v>7.4</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>10.3</v>
+      </c>
+      <c r="H9">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
+        <v>6.2</v>
+      </c>
+      <c r="C10">
+        <v>6.9</v>
+      </c>
+      <c r="D10">
         <v>7.7</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>8.6</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>10.7</v>
+      </c>
+      <c r="H10">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
+        <v>6.4</v>
+      </c>
+      <c r="C11">
+        <v>7.1</v>
+      </c>
+      <c r="D11">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>8.9</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
+        <v>6.6</v>
+      </c>
+      <c r="C12">
+        <v>7.4</v>
+      </c>
+      <c r="D12">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>9.1999999999999993</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>11.4</v>
+      </c>
+      <c r="H12">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
+        <v>6.8</v>
+      </c>
+      <c r="C13">
+        <v>7.6</v>
+      </c>
+      <c r="D13">
         <v>8.4</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>9.4</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>11.7</v>
+      </c>
+      <c r="H13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
+        <v>6.9</v>
+      </c>
+      <c r="C14">
+        <v>7.7</v>
+      </c>
+      <c r="D14">
         <v>8.6</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>9.6</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>10.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
+        <v>7.1</v>
+      </c>
+      <c r="C15">
+        <v>7.9</v>
+      </c>
+      <c r="D15">
         <v>8.8000000000000007</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>9.9</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>12.3</v>
+      </c>
+      <c r="H15">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
+        <v>7.2</v>
+      </c>
+      <c r="C16">
+        <v>8.1</v>
+      </c>
+      <c r="D16">
         <v>9</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>10.1</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>11.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>12.6</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
+        <v>7.4</v>
+      </c>
+      <c r="C17">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D17">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C17">
+      <c r="E17">
         <v>10.3</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>12.8</v>
+      </c>
+      <c r="H17">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
+        <v>7.5</v>
+      </c>
+      <c r="C18">
+        <v>8.4</v>
+      </c>
+      <c r="D18">
         <v>9.4</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>10.5</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>11.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>13.1</v>
+      </c>
+      <c r="H18">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
+        <v>7.7</v>
+      </c>
+      <c r="C19">
+        <v>8.6</v>
+      </c>
+      <c r="D19">
         <v>9.6</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>10.7</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>13.4</v>
+      </c>
+      <c r="H19">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
+        <v>7.8</v>
+      </c>
+      <c r="C20">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D20">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <v>10.9</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>12.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>13.7</v>
+      </c>
+      <c r="H20">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>8.9</v>
+      </c>
+      <c r="D21">
         <v>10</v>
       </c>
-      <c r="C21">
+      <c r="E21">
         <v>11.1</v>
       </c>
-      <c r="D21">
+      <c r="F21">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>13.9</v>
+      </c>
+      <c r="H21">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
+        <v>8.1</v>
+      </c>
+      <c r="C22">
+        <v>9.1</v>
+      </c>
+      <c r="D22">
         <v>10.1</v>
       </c>
-      <c r="C22">
+      <c r="E22">
         <v>11.3</v>
       </c>
-      <c r="D22">
+      <c r="F22">
         <v>12.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>14.2</v>
+      </c>
+      <c r="H22">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C23">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D23">
         <v>10.3</v>
       </c>
-      <c r="C23">
+      <c r="E23">
         <v>11.5</v>
       </c>
-      <c r="D23">
+      <c r="F23">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>14.5</v>
+      </c>
+      <c r="H23">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
+        <v>8.4</v>
+      </c>
+      <c r="C24">
+        <v>9.4</v>
+      </c>
+      <c r="D24">
         <v>10.5</v>
       </c>
-      <c r="C24">
+      <c r="E24">
         <v>11.8</v>
       </c>
-      <c r="D24">
+      <c r="F24">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>14.7</v>
+      </c>
+      <c r="H24">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
+        <v>8.5</v>
+      </c>
+      <c r="C25">
+        <v>9.5</v>
+      </c>
+      <c r="D25">
         <v>10.7</v>
       </c>
-      <c r="C25">
+      <c r="E25">
         <v>12</v>
       </c>
-      <c r="D25">
+      <c r="F25">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>15</v>
+      </c>
+      <c r="H25">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
+        <v>8.6</v>
+      </c>
+      <c r="C26">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D26">
         <v>10.8</v>
       </c>
-      <c r="C26">
+      <c r="E26">
         <v>12.2</v>
       </c>
-      <c r="D26">
+      <c r="F26">
         <v>13.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>15.3</v>
+      </c>
+      <c r="H26">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C27">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D27">
         <v>11</v>
       </c>
-      <c r="C27">
+      <c r="E27">
         <v>12.4</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <v>13.9</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>15.5</v>
+      </c>
+      <c r="H27">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
+        <v>8.9</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28">
         <v>11.2</v>
       </c>
-      <c r="C28">
+      <c r="E28">
         <v>12.5</v>
       </c>
-      <c r="D28">
+      <c r="F28">
         <v>14.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>15.8</v>
+      </c>
+      <c r="H28">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>10.1</v>
+      </c>
+      <c r="D29">
         <v>11.3</v>
       </c>
-      <c r="C29">
+      <c r="E29">
         <v>12.7</v>
       </c>
-      <c r="D29">
+      <c r="F29">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="H29">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
+        <v>9.1</v>
+      </c>
+      <c r="C30">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D30">
         <v>11.5</v>
       </c>
-      <c r="C30">
+      <c r="E30">
         <v>12.9</v>
       </c>
-      <c r="D30">
+      <c r="F30">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>16.3</v>
+      </c>
+      <c r="H30">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C31">
+        <v>10.4</v>
+      </c>
+      <c r="D31">
         <v>11.7</v>
       </c>
-      <c r="C31">
+      <c r="E31">
         <v>13.1</v>
       </c>
-      <c r="D31">
+      <c r="F31">
         <v>14.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="H31">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
+        <v>9.4</v>
+      </c>
+      <c r="C32">
+        <v>10.5</v>
+      </c>
+      <c r="D32">
         <v>11.8</v>
       </c>
-      <c r="C32">
+      <c r="E32">
         <v>13.3</v>
       </c>
-      <c r="D32">
+      <c r="F32">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="H32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
+        <v>9.5</v>
+      </c>
+      <c r="C33">
+        <v>10.7</v>
+      </c>
+      <c r="D33">
         <v>12</v>
       </c>
-      <c r="C33">
+      <c r="E33">
         <v>13.5</v>
       </c>
-      <c r="D33">
+      <c r="F33">
         <v>15.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="H33">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
+        <v>9.6</v>
+      </c>
+      <c r="C34">
+        <v>10.8</v>
+      </c>
+      <c r="D34">
         <v>12.1</v>
       </c>
-      <c r="C34">
+      <c r="E34">
         <v>13.7</v>
       </c>
-      <c r="D34">
+      <c r="F34">
         <v>15.4</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="H34">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C35">
+        <v>10.9</v>
+      </c>
+      <c r="D35">
         <v>12.3</v>
       </c>
-      <c r="C35">
+      <c r="E35">
         <v>13.8</v>
       </c>
-      <c r="D35">
+      <c r="F35">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H35">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C36">
+        <v>11</v>
+      </c>
+      <c r="D36">
         <v>12.4</v>
       </c>
-      <c r="C36">
+      <c r="E36">
         <v>14</v>
       </c>
-      <c r="D36">
+      <c r="F36">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>17.8</v>
+      </c>
+      <c r="H36">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
+        <v>9.9</v>
+      </c>
+      <c r="C37">
+        <v>11.2</v>
+      </c>
+      <c r="D37">
         <v>12.6</v>
       </c>
-      <c r="C37">
+      <c r="E37">
         <v>14.2</v>
       </c>
-      <c r="D37">
+      <c r="F37">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="H37">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>11.3</v>
+      </c>
+      <c r="D38">
         <v>12.7</v>
       </c>
-      <c r="C38">
+      <c r="E38">
         <v>14.3</v>
       </c>
-      <c r="D38">
+      <c r="F38">
         <v>16.2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>18.3</v>
+      </c>
+      <c r="H38">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
+        <v>10.1</v>
+      </c>
+      <c r="C39">
+        <v>11.4</v>
+      </c>
+      <c r="D39">
         <v>12.9</v>
       </c>
-      <c r="C39">
+      <c r="E39">
         <v>14.5</v>
       </c>
-      <c r="D39">
+      <c r="F39">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="H39">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C40">
+        <v>11.5</v>
+      </c>
+      <c r="D40">
         <v>13</v>
       </c>
-      <c r="C40">
+      <c r="E40">
         <v>14.7</v>
       </c>
-      <c r="D40">
+      <c r="F40">
         <v>16.600000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>18.8</v>
+      </c>
+      <c r="H40">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
+        <v>10.3</v>
+      </c>
+      <c r="C41">
+        <v>11.6</v>
+      </c>
+      <c r="D41">
         <v>13.1</v>
       </c>
-      <c r="C41">
+      <c r="E41">
         <v>14.8</v>
       </c>
-      <c r="D41">
+      <c r="F41">
         <v>16.8</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>19</v>
+      </c>
+      <c r="H41">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
+        <v>10.4</v>
+      </c>
+      <c r="C42">
+        <v>11.8</v>
+      </c>
+      <c r="D42">
         <v>13.3</v>
       </c>
-      <c r="C42">
+      <c r="E42">
         <v>15</v>
       </c>
-      <c r="D42">
+      <c r="F42">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>19.3</v>
+      </c>
+      <c r="H42">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43">
+        <v>10.5</v>
+      </c>
+      <c r="C43">
+        <v>11.9</v>
+      </c>
+      <c r="D43">
         <v>13.4</v>
       </c>
-      <c r="C43">
+      <c r="E43">
         <v>15.2</v>
       </c>
-      <c r="D43">
+      <c r="F43">
         <v>17.2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>19.5</v>
+      </c>
+      <c r="H43">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
+        <v>10.6</v>
+      </c>
+      <c r="C44">
+        <v>12</v>
+      </c>
+      <c r="D44">
         <v>13.6</v>
       </c>
-      <c r="C44">
+      <c r="E44">
         <v>15.3</v>
       </c>
-      <c r="D44">
+      <c r="F44">
         <v>17.399999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>19.7</v>
+      </c>
+      <c r="H44">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
+        <v>10.7</v>
+      </c>
+      <c r="C45">
+        <v>12.1</v>
+      </c>
+      <c r="D45">
         <v>13.7</v>
       </c>
-      <c r="C45">
+      <c r="E45">
         <v>15.5</v>
       </c>
-      <c r="D45">
+      <c r="F45">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>20</v>
+      </c>
+      <c r="H45">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46">
+        <v>10.8</v>
+      </c>
+      <c r="C46">
+        <v>12.2</v>
+      </c>
+      <c r="D46">
         <v>13.8</v>
       </c>
-      <c r="C46">
+      <c r="E46">
         <v>15.7</v>
       </c>
-      <c r="D46">
+      <c r="F46">
         <v>17.8</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>20.2</v>
+      </c>
+      <c r="H46">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47">
+        <v>10.9</v>
+      </c>
+      <c r="C47">
+        <v>12.4</v>
+      </c>
+      <c r="D47">
         <v>14</v>
       </c>
-      <c r="C47">
+      <c r="E47">
         <v>15.8</v>
       </c>
-      <c r="D47">
+      <c r="F47">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>20.5</v>
+      </c>
+      <c r="H47">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>12.5</v>
+      </c>
+      <c r="D48">
         <v>14.1</v>
       </c>
-      <c r="C48">
+      <c r="E48">
         <v>16</v>
       </c>
-      <c r="D48">
+      <c r="F48">
         <v>18.2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>20.7</v>
+      </c>
+      <c r="H48">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49">
+        <v>11.1</v>
+      </c>
+      <c r="C49">
+        <v>12.6</v>
+      </c>
+      <c r="D49">
         <v>14.3</v>
       </c>
-      <c r="C49">
+      <c r="E49">
         <v>16.2</v>
       </c>
-      <c r="D49">
+      <c r="F49">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>20.9</v>
+      </c>
+      <c r="H49">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50">
+        <v>11.2</v>
+      </c>
+      <c r="C50">
+        <v>12.7</v>
+      </c>
+      <c r="D50">
         <v>14.4</v>
       </c>
-      <c r="C50">
+      <c r="E50">
         <v>16.3</v>
       </c>
-      <c r="D50">
+      <c r="F50">
         <v>18.600000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>21.2</v>
+      </c>
+      <c r="H50">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51">
+        <v>11.3</v>
+      </c>
+      <c r="C51">
+        <v>12.8</v>
+      </c>
+      <c r="D51">
         <v>14.5</v>
       </c>
-      <c r="C51">
+      <c r="E51">
         <v>16.5</v>
       </c>
-      <c r="D51">
+      <c r="F51">
         <v>18.8</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>21.4</v>
+      </c>
+      <c r="H51">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52">
+        <v>11.4</v>
+      </c>
+      <c r="C52">
+        <v>12.9</v>
+      </c>
+      <c r="D52">
         <v>14.7</v>
       </c>
-      <c r="C52">
+      <c r="E52">
         <v>16.7</v>
       </c>
-      <c r="D52">
+      <c r="F52">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>21.7</v>
+      </c>
+      <c r="H52">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53">
+        <v>11.5</v>
+      </c>
+      <c r="C53">
+        <v>13.1</v>
+      </c>
+      <c r="D53">
         <v>14.8</v>
       </c>
-      <c r="C53">
+      <c r="E53">
         <v>16.8</v>
       </c>
-      <c r="D53">
+      <c r="F53">
         <v>19.2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>21.9</v>
+      </c>
+      <c r="H53">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54">
+        <v>11.6</v>
+      </c>
+      <c r="C54">
+        <v>13.2</v>
+      </c>
+      <c r="D54">
         <v>15</v>
       </c>
-      <c r="C54">
+      <c r="E54">
         <v>17</v>
       </c>
-      <c r="D54">
+      <c r="F54">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>22.2</v>
+      </c>
+      <c r="H54">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55">
+        <v>11.7</v>
+      </c>
+      <c r="C55">
+        <v>13.3</v>
+      </c>
+      <c r="D55">
         <v>15.1</v>
       </c>
-      <c r="C55">
+      <c r="E55">
         <v>17.2</v>
       </c>
-      <c r="D55">
+      <c r="F55">
         <v>19.600000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>22.4</v>
+      </c>
+      <c r="H55">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56">
+        <v>11.8</v>
+      </c>
+      <c r="C56">
+        <v>13.4</v>
+      </c>
+      <c r="D56">
         <v>15.2</v>
       </c>
-      <c r="C56">
+      <c r="E56">
         <v>17.3</v>
       </c>
-      <c r="D56">
+      <c r="F56">
         <v>19.8</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>22.7</v>
+      </c>
+      <c r="H56">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57">
+        <v>11.9</v>
+      </c>
+      <c r="C57">
+        <v>13.5</v>
+      </c>
+      <c r="D57">
         <v>15.4</v>
       </c>
-      <c r="C57">
+      <c r="E57">
         <v>17.5</v>
       </c>
-      <c r="D57">
+      <c r="F57">
         <v>20</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>22.9</v>
+      </c>
+      <c r="H57">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58">
+        <v>12</v>
+      </c>
+      <c r="C58">
+        <v>13.6</v>
+      </c>
+      <c r="D58">
         <v>15.5</v>
       </c>
-      <c r="C58">
+      <c r="E58">
         <v>17.7</v>
       </c>
-      <c r="D58">
+      <c r="F58">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>23.2</v>
+      </c>
+      <c r="H58">
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59">
+        <v>12.1</v>
+      </c>
+      <c r="C59">
+        <v>13.7</v>
+      </c>
+      <c r="D59">
         <v>15.6</v>
       </c>
-      <c r="C59">
+      <c r="E59">
         <v>17.8</v>
       </c>
-      <c r="D59">
+      <c r="F59">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>23.4</v>
+      </c>
+      <c r="H59">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60">
+        <v>12.2</v>
+      </c>
+      <c r="C60">
+        <v>13.8</v>
+      </c>
+      <c r="D60">
         <v>15.8</v>
       </c>
-      <c r="C60">
+      <c r="E60">
         <v>18</v>
       </c>
-      <c r="D60">
+      <c r="F60">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>23.7</v>
+      </c>
+      <c r="H60">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61">
+        <v>12.3</v>
+      </c>
+      <c r="C61">
+        <v>14</v>
+      </c>
+      <c r="D61">
         <v>15.9</v>
       </c>
-      <c r="C61">
+      <c r="E61">
         <v>18.2</v>
       </c>
-      <c r="D61">
+      <c r="F61">
         <v>20.8</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>23.9</v>
+      </c>
+      <c r="H61">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62">
+        <v>12.4</v>
+      </c>
+      <c r="C62">
+        <v>14.1</v>
+      </c>
+      <c r="D62">
         <v>16</v>
       </c>
-      <c r="C62">
+      <c r="E62">
         <v>18.3</v>
       </c>
-      <c r="D62">
+      <c r="F62">
         <v>21</v>
+      </c>
+      <c r="G62">
+        <v>24.2</v>
+      </c>
+      <c r="H62">
+        <v>27.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>